<commit_message>
In this commit App has a new things both vulnerability and source code. At vulnerability side it have new Idor at ListFile, Account takover at Update User and basic JWT Secret used. About code side Basic Authentication component add Swagger page, Endpoint named change less format and also for UI side Refresh token endpoint is created and control. So that changes is effect also dummy_data.py script
</commit_message>
<xml_diff>
--- a/Resource/Vulnerabilityinfo/VulnerableAppForAPIVulnerabilityList.xlsx
+++ b/Resource/Vulnerabilityinfo/VulnerableAppForAPIVulnerabilityList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vakifbank/Desktop/VulnerableApp4APISecurity/Resource/Vulnerabilityinfo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vakifbank/RiderProjects/VulnerableApp4APISecurity/Resource/Vulnerabilityinfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8F6CC8-FE45-884E-8C62-E0EBADCD7915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C91448-ADED-8340-BDBD-90665D4FF53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20940" xr2:uid="{3D987C12-2CEC-194B-B129-D4CA5F7B8D9A}"/>
+    <workbookView xWindow="17620" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{3D987C12-2CEC-194B-B129-D4CA5F7B8D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Account/Login</t>
   </si>
@@ -47,57 +46,9 @@
     <t>Account/Register</t>
   </si>
   <si>
-    <t>Account/GetAccount</t>
-  </si>
-  <si>
-    <t>Account/UpdateNameAndSurnameAccount</t>
-  </si>
-  <si>
-    <t>Account/GetAccounts</t>
-  </si>
-  <si>
-    <t>Account/DeleteAccount</t>
-  </si>
-  <si>
-    <t>Card/GetCard</t>
-  </si>
-  <si>
-    <t>Card/GetCardV2</t>
-  </si>
-  <si>
-    <t>Card/CreateCard</t>
-  </si>
-  <si>
-    <t>Card/DeleteCard</t>
-  </si>
-  <si>
-    <t>Helper/ShowPorfileAsHtmlFormat</t>
-  </si>
-  <si>
     <t>Helper/SystemDate</t>
   </si>
   <si>
-    <t>Helper/ListUploadedeFile</t>
-  </si>
-  <si>
-    <t>Helper/DowloadImageFromRemote</t>
-  </si>
-  <si>
-    <t>Helper/DowloadImageFromLocale</t>
-  </si>
-  <si>
-    <t>Profile/GetProfile</t>
-  </si>
-  <si>
-    <t>Profile/CreateProfile</t>
-  </si>
-  <si>
-    <t>Profile/UpdateProfile</t>
-  </si>
-  <si>
-    <t>Profile/DeleteProfile</t>
-  </si>
-  <si>
     <t>Endpoint</t>
   </si>
   <si>
@@ -116,9 +67,6 @@
     <t>Mass Assigment, Email Detect</t>
   </si>
   <si>
-    <t xml:space="preserve"> - </t>
-  </si>
-  <si>
     <t>After Fuzzing User can use administrator endpoint</t>
   </si>
   <si>
@@ -146,12 +94,6 @@
     <t>SSRF</t>
   </si>
   <si>
-    <t>Generate error message</t>
-  </si>
-  <si>
-    <t>Show Input Violation bug as a html content, Excessive data exposure from password</t>
-  </si>
-  <si>
     <t>LFI, Directory Traversal</t>
   </si>
   <si>
@@ -176,9 +118,6 @@
     <t>API 05:2019 — Broken function level authorization</t>
   </si>
   <si>
-    <t>API 07:2019 — Security misconfiguration</t>
-  </si>
-  <si>
     <t>API 08:2019 — Injection</t>
   </si>
   <si>
@@ -195,6 +134,93 @@
   </si>
   <si>
     <t>API 01:2019 — Broken object level authorization - Kontrol et</t>
+  </si>
+  <si>
+    <t>Account/RefreshToken</t>
+  </si>
+  <si>
+    <t>Account/TokenStatus</t>
+  </si>
+  <si>
+    <t>GET - User/</t>
+  </si>
+  <si>
+    <t>PUT - User/</t>
+  </si>
+  <si>
+    <t>IDOR/BOLA from Email and Account Takeover, Input Violation</t>
+  </si>
+  <si>
+    <t>API 01:2019 - Broken object level authorization, API 08:2019 - Injection</t>
+  </si>
+  <si>
+    <t>DELETE - User/</t>
+  </si>
+  <si>
+    <t>User/Users</t>
+  </si>
+  <si>
+    <t>Vulnerability = Excessive data Exposure with show Credit Card Number and Card Password.</t>
+  </si>
+  <si>
+    <t>API 02:2019 - Broken authentication, API 07:2019 - Security misconfiguration.</t>
+  </si>
+  <si>
+    <t>GET - Profile/</t>
+  </si>
+  <si>
+    <t>POST - Profile/</t>
+  </si>
+  <si>
+    <t>PUT - Profile/</t>
+  </si>
+  <si>
+    <t>DELETE - Profile/</t>
+  </si>
+  <si>
+    <t>Profile/ShowUserProfile</t>
+  </si>
+  <si>
+    <t>Input Violation and Excessive data Exposure with show password</t>
+  </si>
+  <si>
+    <t>API 08:2019 — Injection, API 03:2019 — Excessive data exposure</t>
+  </si>
+  <si>
+    <t>GET - Card/GetCardV2</t>
+  </si>
+  <si>
+    <t>POST - Card/</t>
+  </si>
+  <si>
+    <t>DELETE - Card/</t>
+  </si>
+  <si>
+    <t>GET - Card/</t>
+  </si>
+  <si>
+    <t>Helper/ShowLog</t>
+  </si>
+  <si>
+    <t>Helper/ListFile</t>
+  </si>
+  <si>
+    <t>Un authenticated request.</t>
+  </si>
+  <si>
+    <t>API 02:2019 - Broken authentication, API 03:2019 - Excessive data exposure, API 04:2019 - Lack of resources and rate limiting</t>
+  </si>
+  <si>
+    <t>List uploaded file by name so IDOR/BOLA</t>
+  </si>
+  <si>
+    <t>API 01:2019 - Broken object level authorization</t>
+  </si>
+  <si>
+    <t>Helper/GetImageFromRemote</t>
+  </si>
+  <si>
+    <t>Helper/GetImageFromLocale</t>
   </si>
 </sst>
 </file>
@@ -238,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +289,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -310,15 +341,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
@@ -354,8 +386,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Accent2" xfId="6" builtinId="33"/>
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Accent5" xfId="5" builtinId="45"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -673,7 +716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B09439-701E-2546-B3F5-65CEEF43887A}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="141" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -682,20 +725,20 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,10 +746,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -714,10 +757,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -725,221 +768,255 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>